<commit_message>
CCDI Studies as of 04/17 11am
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC01_CCDI_phs000468.xlsx
+++ b/InputFiles/CCDI/TC01_CCDI_phs000468.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation\sowjanya0307\Commons_Automation\InputFiles\CCDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A986D1E-2276-412F-99C0-215B141D4A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514F4664-69B9-4DF7-AB49-A8BE48847A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="165" windowWidth="28800" windowHeight="15435" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -158,30 +158,6 @@
 left join funding f on s.study_id = f.study </t>
   </si>
   <si>
-    <t>SELECT DISTINCT
-   smp.sample_id AS "Sample ID",
-    prt.participant_id AS "Participant ID", std.dbgap_accession AS "Study ID" , std.id, smp.anatomic_site AS "Sample Anatomic Site", dgn. "participant.id",
-    COALESCE(CASE WHEN smp.participant_age_at_collection = -999 THEN 'Not Reported' ELSE smp.participant_age_at_collection END, 0) AS "Age at Sample Collection (days)",
-    COALESCE(smp.sample_tumor_status, '') AS "Sample Tumor Status",
-    COALESCE(smp.tumor_classification, '') AS "Sample Tumor Classification",
---COALESCE(CASE WHEN dgn."participant.id" is null THEN dgn.diagnosis ELSE dgn.diagnosis_comment END,dgn.diagnosis_comment) AS "Sample Diagnosis1",
- dgn.diagnosis as "Sample Diagnosis"
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_sample smp ON prt.id = smp."participant.id"
-LEFT JOIN 
-    df_diagnosis dgn ON smp."id" = dgn."sample.id"
-WHERE 
-   std.dbgap_accession = 'phs000468' 
-AND smp.sample_id IS NOT NULL
-ORDER BY 
-   smp.sample_id ASC
-;</t>
-  </si>
-  <si>
     <t>with file_data as (
 select file_name, data_category, file_type, file_size, file_access, file_description,"study.id" studyid, "participant.id" as participantid from df_clinical_measure_file )
 SELECT fd.file_name AS "File Name",
@@ -205,6 +181,29 @@
     file_data fd ON std.id = fd.studyid
 WHERE 
     std.dbgap_accession = 'phs000468'</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT
+   smp.sample_id AS "Sample ID",
+    prt.participant_id AS "Participant ID", std.dbgap_accession AS "Study ID", smp.anatomic_site AS "Sample Anatomic Site",
+    COALESCE(CASE WHEN smp.participant_age_at_collection = -999 THEN 'Not Reported' ELSE smp.participant_age_at_collection END, 0) AS "Age at Sample Collection (days)",
+    COALESCE(smp.sample_tumor_status, '') AS "Sample Tumor Status",
+    COALESCE(smp.tumor_classification, '') AS "Sample Tumor Classification",
+ dgn.diagnosis as "Sample Diagnosis"
+FROM 
+    df_study std
+LEFT JOIN 
+    df_participant prt ON std.id = prt."study.id"
+LEFT JOIN 
+    df_sample smp ON prt.id = smp."participant.id"
+LEFT JOIN 
+    df_diagnosis dgn ON smp."id" = dgn."sample.id"
+WHERE 
+   std.dbgap_accession = 'phs000468' 
+AND smp.sample_id IS NOT NULL
+ORDER BY 
+   smp.sample_id ASC
+;</t>
   </si>
 </sst>
 </file>
@@ -606,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,12 +660,12 @@
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="378" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -675,7 +674,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2"/>
     </row>

</xml_diff>